<commit_message>
Changed indexing and > 1 slack
Now there are no calculations like pq-1 and the code contemplates more than 1 slack. Some testing should be done
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z\Desktop\Josep\PycharmProjects\Complet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOSEP\Desktop\TFG\Codi\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Busos" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>R</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Slack</t>
+  </si>
+  <si>
+    <t>delta</t>
   </si>
 </sst>
 </file>
@@ -119,7 +122,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -381,15 +384,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -403,21 +406,27 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -427,11 +436,11 @@
       <c r="C3">
         <v>-0.1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -441,11 +450,11 @@
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -455,11 +464,11 @@
       <c r="C5">
         <v>-0.1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -469,11 +478,11 @@
       <c r="D6">
         <v>0.95</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -483,11 +492,11 @@
       <c r="D7">
         <v>0.94</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -497,11 +506,11 @@
       <c r="C8">
         <v>-7.0000000000000007E-2</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -511,11 +520,11 @@
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -525,11 +534,11 @@
       <c r="D10">
         <v>0.91</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -539,11 +548,11 @@
       <c r="C11">
         <v>-0.05</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -553,11 +562,11 @@
       <c r="D12">
         <v>0.98</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -567,8 +576,22 @@
       <c r="D13">
         <v>0.92</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0.1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -578,13 +601,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -841,6 +864,23 @@
         <v>1E-4</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>0.01</v>
+      </c>
+      <c r="D16">
+        <v>0.05</v>
+      </c>
+      <c r="E16">
+        <v>1E-4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added script to convert the grids to GridCal format
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,46 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOSEP\Desktop\TFG\Codi\Tests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView windowWidth="7365" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="Busos" sheetId="1" r:id="rId1"/>
     <sheet name="Topologia" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Busos!$A$1:$F$17</definedName>
+  </definedNames>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>B/2</t>
-  </si>
-  <si>
-    <t>Bus fi</t>
-  </si>
-  <si>
-    <t>Bus inici</t>
-  </si>
   <si>
     <t>Bus</t>
   </si>
@@ -54,10 +33,10 @@
     <t>V</t>
   </si>
   <si>
-    <t>Tipus</t>
+    <t>delta</t>
   </si>
   <si>
-    <t>PV</t>
+    <t>Tipus</t>
   </si>
   <si>
     <t>PQ</t>
@@ -66,31 +45,382 @@
     <t>Slack</t>
   </si>
   <si>
-    <t>delta</t>
+    <t>PV</t>
+  </si>
+  <si>
+    <t>Bus inici</t>
+  </si>
+  <si>
+    <t>Bus fi</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>B/2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -98,24 +428,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -164,7 +780,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -199,7 +815,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -373,46 +989,41 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="14.25" outlineLevelCol="5"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>0</v>
       </c>
@@ -422,11 +1033,14 @@
       <c r="C2">
         <v>-0.1</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
       <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1</v>
       </c>
@@ -437,10 +1051,10 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>2</v>
       </c>
@@ -450,11 +1064,14 @@
       <c r="C4">
         <v>0</v>
       </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
       <c r="F4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>3</v>
       </c>
@@ -464,11 +1081,14 @@
       <c r="C5">
         <v>-0.1</v>
       </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
       <c r="F5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>4</v>
       </c>
@@ -479,10 +1099,10 @@
         <v>0.95</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>5</v>
       </c>
@@ -493,10 +1113,10 @@
         <v>0.94</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>6</v>
       </c>
@@ -504,13 +1124,16 @@
         <v>-0.1</v>
       </c>
       <c r="C8">
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.07</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>7</v>
       </c>
@@ -520,11 +1143,14 @@
       <c r="C9">
         <v>0</v>
       </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
       <c r="F9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>8</v>
       </c>
@@ -535,10 +1161,10 @@
         <v>0.91</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>9</v>
       </c>
@@ -548,11 +1174,14 @@
       <c r="C11">
         <v>-0.05</v>
       </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
       <c r="F11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>10</v>
       </c>
@@ -563,10 +1192,10 @@
         <v>0.98</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>11</v>
       </c>
@@ -577,10 +1206,10 @@
         <v>0.92</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>12</v>
       </c>
@@ -588,13 +1217,13 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>13</v>
       </c>
@@ -604,11 +1233,14 @@
       <c r="C15">
         <v>0</v>
       </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
       <c r="F15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>14</v>
       </c>
@@ -619,10 +1251,10 @@
         <v>0.93</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>15</v>
       </c>
@@ -632,43 +1264,51 @@
       <c r="C17">
         <v>-0.1</v>
       </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
       <c r="F17" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F17">
+    <extLst/>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="A11" sqref="$A11:$XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="14.25" outlineLevelCol="4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -685,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -702,7 +1342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>0</v>
       </c>
@@ -716,10 +1356,10 @@
         <v>0.1</v>
       </c>
       <c r="E4">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>0</v>
       </c>
@@ -733,10 +1373,10 @@
         <v>0.12</v>
       </c>
       <c r="E5">
-        <v>2.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>2</v>
       </c>
@@ -753,7 +1393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>2</v>
       </c>
@@ -770,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>3</v>
       </c>
@@ -784,10 +1424,10 @@
         <v>0.11</v>
       </c>
       <c r="E8">
-        <v>5.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>0</v>
       </c>
@@ -804,7 +1444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>2</v>
       </c>
@@ -821,7 +1461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>7</v>
       </c>
@@ -838,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>4</v>
       </c>
@@ -852,10 +1492,10 @@
         <v>0.05</v>
       </c>
       <c r="E12">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>0</v>
       </c>
@@ -866,13 +1506,13 @@
         <v>0.01</v>
       </c>
       <c r="D13">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>10</v>
       </c>
@@ -889,7 +1529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>5</v>
       </c>
@@ -897,16 +1537,16 @@
         <v>11</v>
       </c>
       <c r="C15">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="D15">
         <v>0.05</v>
       </c>
       <c r="E15">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>5</v>
       </c>
@@ -920,10 +1560,10 @@
         <v>0.05</v>
       </c>
       <c r="E16">
-        <v>1E-4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>12</v>
       </c>
@@ -931,16 +1571,16 @@
         <v>13</v>
       </c>
       <c r="C17">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="D17">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>13</v>
       </c>
@@ -954,10 +1594,10 @@
         <v>0.05</v>
       </c>
       <c r="E18">
-        <v>2.0000000000000001E-4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0.0002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>9</v>
       </c>
@@ -965,7 +1605,7 @@
         <v>15</v>
       </c>
       <c r="C19">
-        <v>1.4E-2</v>
+        <v>0.014</v>
       </c>
       <c r="D19">
         <v>0.06</v>
@@ -974,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>13</v>
       </c>
@@ -993,5 +1633,22 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
No numba in convolutions
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOSEP\Desktop\TFG\Codi\HE_Josep\Holomorphic-Embedding-Josep\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="7365" windowHeight="8220"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7365" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="Busos" sheetId="1" r:id="rId1"/>
@@ -66,14 +71,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,346 +80,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -428,310 +97,24 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -989,19 +372,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="14.25" outlineLevelCol="5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -1124,7 +507,7 @@
         <v>-0.1</v>
       </c>
       <c r="C8">
-        <v>-0.07</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1272,24 +655,20 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F17">
-    <extLst/>
-  </autoFilter>
+  <autoFilter ref="A1:F17"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="$A11:$XFD11"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="14.25" outlineLevelCol="4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -1356,7 +735,7 @@
         <v>0.1</v>
       </c>
       <c r="E4">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1373,7 +752,7 @@
         <v>0.12</v>
       </c>
       <c r="E5">
-        <v>0.0002</v>
+        <v>2.0000000000000001E-4</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1424,7 +803,7 @@
         <v>0.11</v>
       </c>
       <c r="E8">
-        <v>0.0005</v>
+        <v>5.0000000000000001E-4</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1492,7 +871,7 @@
         <v>0.05</v>
       </c>
       <c r="E12">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1506,7 +885,7 @@
         <v>0.01</v>
       </c>
       <c r="D13">
-        <v>0.07</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1537,13 +916,13 @@
         <v>11</v>
       </c>
       <c r="C15">
-        <v>0.015</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D15">
         <v>0.05</v>
       </c>
       <c r="E15">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1560,7 +939,7 @@
         <v>0.05</v>
       </c>
       <c r="E16">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1571,10 +950,10 @@
         <v>13</v>
       </c>
       <c r="C17">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D17">
-        <v>0.07</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1594,7 +973,7 @@
         <v>0.05</v>
       </c>
       <c r="E18">
-        <v>0.0002</v>
+        <v>2.0000000000000001E-4</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1605,7 +984,7 @@
         <v>15</v>
       </c>
       <c r="C19">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
       <c r="D19">
         <v>0.06</v>
@@ -1633,22 +1012,17 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>